<commit_message>
added log for bicu
</commit_message>
<xml_diff>
--- a/template/log.xlsx
+++ b/template/log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Program\excel_worker\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED32AE5C-7A3F-42C2-BA8C-272C5370A524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BBC97A-E6AE-481F-8819-F0807FD1CA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="1" r:id="rId1"/>
@@ -115,26 +115,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,89 +453,89 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="41" style="4" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="27" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" style="4" customWidth="1"/>
-    <col min="11" max="12" width="10.85546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="41" style="3" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="27" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" style="3" customWidth="1"/>
+    <col min="11" max="12" width="10.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="3" t="s">
+      <c r="I1" s="6"/>
+      <c r="J1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="6" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
add consumer hash and network hash
</commit_message>
<xml_diff>
--- a/template/log.xlsx
+++ b/template/log.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Program\excel_worker\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BBC97A-E6AE-481F-8819-F0807FD1CA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56E60AE-7EC5-4950-9BD5-613D912DB478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0" refMode="R1C1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -138,7 +138,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -154,9 +154,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -194,7 +194,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -300,7 +300,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -453,7 +453,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>